<commit_message>
Add large file to Git LFS tracking
</commit_message>
<xml_diff>
--- a/src/utnce/check_name.xlsx
+++ b/src/utnce/check_name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A120"/>
+  <dimension ref="A1:A116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,15 +469,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>osm_id                                               13649635
-route                                                     bus
-to                                   Slikkerveer, Sporttunnel
-name        Bus 142: Rotterdam Zuidplein =&gt; Slikkerveer Sp...
-ref                                                       142
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4891393 51.8876688, 4.4890...
-Name: 4, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -533,15 +525,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>osm_id                                               13206952
-route                                                     bus
-to                                         Dordrecht, Station
-name        Bus 145: Rotterdam Kralingse Zoom =&gt; Dordrecht...
-ref                                                       145
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.5325838 51.9218251, 4.5327...
-Name: 12, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -604,15 +588,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>osm_id                                                 383405
-route                                                     bus
-to                         Lansingerland-Zoetermeer Zuidplein
-name        Bus 173: Berkel en Rodenrijs Rodenrijs Metro =...
-ref                                                       173
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4616458 51.9758184, 4.4618...
-Name: 21, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -675,15 +651,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>osm_id                                                1755250
-route                                                     bus
-to                                    Ridderkerk, Donkersloot
-name        Bus 290: Rotterdam Zuidplein =&gt; Ridderkerk Don...
-ref                                                       290
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4891393 51.8876688, 4.4890...
-Name: 30, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -830,15 +798,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>osm_id                                                 384325
-route                                                     bus
-to                                     Rotterdam, Caïrostraat
-name        Bus 42: Rotterdam Marconiplein =&gt; Rotterdam Be...
-ref                                                        42
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4316822 51.9136058, 4.4318...
-Name: 51, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -887,15 +847,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>osm_id                                                 384661
-route                                                     bus
-to                                Schiedam, Nieuwe Maasstraat
-name           Bus 54: Schiedam Centrum =&gt; Schiedam De Gorzen
-ref                                                        54
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4090742 51.9213762, 4.4084...
-Name: 58, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -909,15 +861,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>osm_id                                                 384341
-route                                                     bus
-to                                   Rotterdam, Meeuwenstaart
-name        Bus 547: Rotterdam Noordereiland =&gt; Rotterdam ...
-ref                                                       547
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4887007 51.9098734, 4.4885...
-Name: 60, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1001,15 +945,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>osm_id                                                6397486
-route                                                     bus
-to                                    Barendrecht, Station NS
-name        Bus 608: Ridderkerk Olmenlaan =&gt; Barendrecht S...
-ref                                                       608
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.5820072 51.8725648, 4.5826...
-Name: 72, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1044,15 +980,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>osm_id                                               13647647
-route                                                     bus
-to                                    Barendrecht, Station NS
-name        Bus 610: Ridderkerk Koningsplein =&gt; Barendrech...
-ref                                                       610
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.600817 51.8708585, 4.60088...
-Name: 77, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1115,30 +1043,14 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>osm_id                                                 384833
-route                                                     bus
-to                                       Rotterdam, Damstraat
-name        Bus 66: Rotterdam Zuidplein =&gt; Rotterdam Feije...
-ref                                                        66
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4890851 51.8875527, 4.4889...
-Name: 86, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>osm_id                                               15797231
-route                                                     bus
-to                                Rotterdam, Antony Fokkerweg
-name        Bus 668: Rotterdam Slinge =&gt; Rotterdam STC Campus
-ref                                                       668
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4780762 51.8746273, 4.4779...
-Name: 87, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1152,15 +1064,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>osm_id                                                9563898
-route                                                     bus
-to                                Rotterdam, Antony Fokkerweg
-name        Bus 668: Rotterdam Zuidplein =&gt; Rotterdam STC ...
-ref                                                       668
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4894556 51.8882072, 4.4894...
-Name: 89, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1202,15 +1106,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>osm_id                                                 385080
-route                                                     bus
-to                                    Rotterdam, Metro Pernis
-name        Bus 69: Rotterdam Zuidplein =&gt; Rotterdam Metro...
-ref                                                        69
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4894216 51.8881435, 4.4892...
-Name: 95, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1231,15 +1127,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>osm_id                                               12125243
-route                                                     bus
-to                                    Rotterdam, Metro Pernis
-name        Bus 69: Rotterdam Zuidplein =&gt; Rotterdam Metro...
-ref                                                        69
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4894216 51.8881435, 4.4892...
-Name: 98, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1309,15 +1197,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>osm_id                                                 385109
-route                                                     bus
-to                                    Rotterdam, SS Rotterdam
-name        Bus 77: Rotterdam Zuidplein =&gt; Rotterdam Katen...
-ref                                                        77
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4890851 51.8875527, 4.4889...
-Name: 108, dtype: object</t>
+          <t>no need to revise</t>
         </is>
       </c>
     </row>
@@ -1358,50 +1238,6 @@
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>osm_id                                                6308493
-route                                                     bus
-to                                       Barendrecht, Station
-name        Bus 84: Rotterdam Zuidplein =&gt; Barendrecht Sta...
-ref                                                        84
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.4891087 51.8876119, 4.4889...
-Name: 115, dtype: object</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>osm_id                                                 382748
-route                                                     bus
-to                                     Rotterdam, Capelsebrug
-name        Bus 97: Rotterdam Capelsebrug =&gt; Krimpen aan d...
-ref                                                        97
-network                                         Bus Rotterdam
-service                                                  None
-geometry    MULTILINESTRING ((4.5578975 51.9211507, 4.5575...
-Name: 117, dtype: object</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
         <is>
           <t>no need to revise</t>
         </is>

</xml_diff>

<commit_message>
rotterdam bus-run shortest path pairs,get buffer
</commit_message>
<xml_diff>
--- a/src/utnce/check_name.xlsx
+++ b/src/utnce/check_name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A116"/>
+  <dimension ref="A1:A109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1194,55 +1194,6 @@
         </is>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>no need to revise</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>